<commit_message>
Changement camera et decor
</commit_message>
<xml_diff>
--- a/divers/backlog.xlsx
+++ b/divers/backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Tache</t>
   </si>
@@ -70,9 +70,6 @@
     <t xml:space="preserve">Ajouter des éléments de décor </t>
   </si>
   <si>
-    <t>Designe Barre de vie : style mortal kombat X</t>
-  </si>
-  <si>
     <t>Zoom progressif sur joueur gagnant</t>
   </si>
   <si>
@@ -140,6 +137,12 @@
   </si>
   <si>
     <t>Ajouter animation de rechargement</t>
+  </si>
+  <si>
+    <t>Coup corps à corps</t>
+  </si>
+  <si>
+    <t>Design Barre de vie : style mortal kombat X</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -508,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
@@ -537,7 +540,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -545,7 +548,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -581,7 +584,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -649,7 +652,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -657,7 +660,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -669,21 +672,21 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -692,12 +695,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -705,7 +708,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -713,7 +716,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -725,7 +728,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -733,7 +736,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -742,12 +745,12 @@
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -755,7 +758,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -763,7 +766,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -771,7 +774,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -779,7 +782,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -811,11 +814,79 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>

</xml_diff>

<commit_message>
Ajout detection area pour eviter que les balles ne traversent les murs
</commit_message>
<xml_diff>
--- a/divers/backlog.xlsx
+++ b/divers/backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Tache</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Réaliser animation player 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Ajouter des éléments de décor </t>
-  </si>
-  <si>
     <t>Zoom progressif sur joueur gagnant</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Design Barre de vie : style mortal kombat X</t>
+  </si>
+  <si>
+    <t>Ajouter des éléments de décor destructibles</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
@@ -540,7 +540,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -548,7 +548,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -652,7 +652,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -660,7 +660,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -672,21 +672,21 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -695,12 +695,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -708,7 +708,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -716,7 +716,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -736,7 +736,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -745,12 +745,12 @@
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -758,7 +758,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -766,7 +766,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -782,7 +782,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -814,15 +814,19 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>

</xml_diff>